<commit_message>
config file path now needs to be passed as an arg
</commit_message>
<xml_diff>
--- a/app/outputs/configuration.xlsx
+++ b/app/outputs/configuration.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="interfaces" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="firewall_objects" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +19,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +47,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -423,4 +437,1192 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>snmp-index</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>role</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>lldp-reception</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>outbandwidth</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>allowaccess</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>vdom</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>interface</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>static</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ip</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>lldp-transmission</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>members</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>fortilink</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>device-identification</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>wan</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>198000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>physical</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ping fgfm</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>wan1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>wan</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>198000</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>physical</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ping fgfm</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>wan2</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>dhcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>dmz</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>physical</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ping https fgfm fabric</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>dmz</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>10.10.10.1 255.255.255.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>physical</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>internal1</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>"To-LAN"</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>physical</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>internal2</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>"To-LAN"</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>physical</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>ping https ssh http fgfm fabric</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>internal3</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>100.64.24.237 255.255.255.252</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>"FortiExtender"</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>physical</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>internal4</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>physical</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>internal5</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>physical</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>physical</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>physical</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>modem</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>pppoe</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>tunnel</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>ssl.root</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>lan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>hard-switch</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>ping https ssh fgfm fabric</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>internal</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>192.168.1.99 255.255.255.0</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>aggregate</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>ping fabric</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>fortilink</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>169.254.1.1 255.255.255.0</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>a" "b</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>loopback</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>ping https ssh snmp</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>loopback0</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>100.64.24.5 255.255.255.255</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>lan</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>ping</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>ipwan1</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>100.66.11.22 255.255.255.252</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>wan</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>ping</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>dia2</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>89.147.120.215 255.255.255.254</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>lan</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>ping</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>ipwan2</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>100.66.11.26 255.255.255.252</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>wan</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>fext-wan</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>fex1</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>dhcp</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>tunnel</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>ping</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>au02-vp-02</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>100.66.11.134 255.255.255.255</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>tunnel</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>ping</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>au04-vp-01</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>100.66.11.166 255.255.255.255</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>lan</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>aggregate</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>ping</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>lag0</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>192.168.5.1 255.255.255.0</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>internal1" "internal2</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>wan</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>ping</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>root</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>dia1</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>89.147.120.213 255.255.255.254</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>uuid</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>associated-interface</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>subnet</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>7a742462-c13a-51ec-12cb-aca6cd89acf1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>154aeb56-c6bd-51ec-c4d1-65232770be4c</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>"FIREWALL_AUTH_PORTAL_ADDRESS"</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>154af4ac-c6bd-51ec-76c3-27c06cf279bb</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>"FABRIC_DEVICE"</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>154d08b4-c6bd-51ec-61c0-b9ff10463e07</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>"SSLVPN_TUNNEL_ADDR1"</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>"ssl.root"</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>iprange</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>17ed18fa-c7c3-51ec-50c1-c283f73dbe8c</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>"FCTEMS_ALL_FORTICLOUD_SERVERS"</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>dynamic</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ea5b02fe-e87d-51ec-45de-1058c8dc3015</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>"nw-ap01"</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>192.168.7.10 255.255.255.255</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>f55a2360-e87d-51ec-a5d9-f95c9392cb67</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>"nw-ap02"</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>192.168.7.11 255.255.255.255</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>017a06d8-e87e-51ec-ab97-93410a582ec4</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>"nw-ap03"</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>192.168.7.13 255.255.255.255</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>0ba7bf88-e87e-51ec-76cc-c7cc7b08155b</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>"nw-ap04"</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>192.168.7.14 255.255.255.255</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>17a955da-e87e-51ec-e257-f807bbfdb39b</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>"nw-ap05"</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>192.168.7.15 255.255.255.255</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>265076fe-e87e-51ec-ecc0-4471a7f569c0</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>"nw-ap06"</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>192.168.7.16 255.255.255.255</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2e109428-e87e-51ec-6083-96f05f3296af</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>"nw-ap07"</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>192.168.7.17 255.255.255.255</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>